<commit_message>
1 Clase taller JS - POO con JavaScript
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ig\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALEXANDER HM\OneDrive\Escritorio\FunzerBitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0323590C-BE59-4C81-B9A1-81CF366247D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Fecha</t>
   </si>
@@ -46,11 +45,17 @@
   <si>
     <t xml:space="preserve">Bitácora diaria Funzer </t>
   </si>
+  <si>
+    <t>Estudio de POO:Elementos(Modelo, Atributos, Comportamiento, Objetos), Pilares(Encapsulamiento, Abstraccion, Herencia, Polimorfismo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se realizan ejercicios para la comprension de programación orientada a objetos en el taller se aplico el aprendizaje teorico de componente y pilares de la POO </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,16 +175,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,6 +187,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -503,11 +514,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E5" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +529,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -526,305 +537,348 @@
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7">
+        <v>44732</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="3:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="3:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="3:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="3:5" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="3:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="3:5" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="3:5" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="3:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="3:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" spans="3:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
     </row>
     <row r="42" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
     </row>
     <row r="44" spans="3:5" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
     </row>
     <row r="46" spans="3:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
     </row>
     <row r="52" spans="3:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
     </row>
     <row r="54" spans="3:5" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
     </row>
     <row r="58" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -835,60 +889,23 @@
     <mergeCell ref="C43:C44"/>
     <mergeCell ref="D43:D44"/>
     <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Notificacion de tareas diarias
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -1,30 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALEXANDER HM\OneDrive\Escritorio\FunzerBitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48B10B9F-7A7D-44CA-AE70-BC21FCCD460C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">Bitácora diaria Funzer </t>
+  </si>
+  <si>
+    <t>Avanze del curso</t>
+  </si>
   <si>
     <t>Fecha</t>
   </si>
@@ -32,53 +49,53 @@
     <t xml:space="preserve">Comentarios </t>
   </si>
   <si>
-    <t>Avanze del curso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bitácora diaria Funzer </t>
-  </si>
-  <si>
     <t>Estudio de POO:Elementos(Modelo, Atributos, Comportamiento, Objetos), Pilares(Encapsulamiento, Abstraccion, Herencia, Polimorfismo)</t>
   </si>
   <si>
+    <t xml:space="preserve">Se realizan ejercicios para la comprension de programación orientada a objetos en el taller se aplico el aprendizaje teorico de componentes y pilares de la POO </t>
+  </si>
+  <si>
+    <t>Capacitacion de Paquete de modulos WebPacket Parte 1</t>
+  </si>
+  <si>
+    <t>Capacitacion referente ala Introduccion a WebPack.En este taller se trabajo sobre el proyecto WebPacket creado en Node.js.Dentro de esta primera parte se encontro una introduccion acerca de los paquetes y modulos quepermiten empaquetar varios archivos con el fin empaquetar todos los componentes de nuestra aplicacion o pagina web</t>
+  </si>
+  <si>
+    <t>Capacitacion de Paquete de modulos WebPacket Parte 2</t>
+  </si>
+  <si>
+    <t>Trabajo sobre un peuqeño ejercicio  que permite enviar un salud, utilizando archivos .js y .html.Configuracion de archivo WebPack.config.js en modo desarrollador.</t>
+  </si>
+  <si>
+    <t>Capacitacion de Paquete de modulos WebPacket Parte 3</t>
+  </si>
+  <si>
+    <t>Configuracion del Servidor de Desarrollo</t>
+  </si>
+  <si>
+    <t>Capacitacion en Github, manejo de repositorios para el desarrollo de backend desde el dispositivo local.</t>
+  </si>
+  <si>
+    <t>Se aprendio sobres los comando basicos de Git, entre los cuales los mas frecuentes son PUSH, COMMIT, PUSH, RESET,  además se creo las ramas principales correctamente para empezar a desarrollar para asi obtener un mejor control de todos los cambios que se vayan realizando.</t>
+  </si>
+  <si>
+    <t>Taller JavaScript Basico-6 JS-JavaScript Basico</t>
+  </si>
+  <si>
     <t>Refuerzo de declaracion de variables, tipos de datos, conversión de datos, practica de suma de numeros, diferentes tipos de operadores, refuerzo de teoria con video tutoriales, instalacion de node js, refuerzo de html.</t>
   </si>
   <si>
-    <t>Capacitacion de Paquete de modulos WebPacket Parte 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se realizan ejercicios para la comprension de programación orientada a objetos en el taller se aplico el aprendizaje teorico de componentes y pilares de la POO </t>
-  </si>
-  <si>
-    <t>Capacitacion referente ala Introduccion a WebPack.En este taller se trabajo sobre el proyecto WebPacket creado en Node.js.Dentro de esta primera parte se encontro una introduccion acerca de los paquetes y modulos quepermiten empaquetar varios archivos con el fin empaquetar todos los componentes de nuestra aplicacion o pagina web</t>
-  </si>
-  <si>
-    <t>Capacitacion de Paquete de modulos WebPacket Parte 2</t>
-  </si>
-  <si>
-    <t>Trabajo sobre un peuqeño ejercicio  que permite enviar un salud, utilizando archivos .js y .html.Configuracion de archivo WebPack.config.js en modo desarrollador.</t>
-  </si>
-  <si>
-    <t>Capacitacion de Paquete de modulos WebPacket Parte 3</t>
-  </si>
-  <si>
-    <t>Configuracion del Servidor de Desarrollo</t>
-  </si>
-  <si>
-    <t>Capacitacion en Github, manejo de repositorios para el desarrollo de backend desde el dispositivo local.</t>
-  </si>
-  <si>
-    <t>Se aprendio sobres los comando basicos de Git, entre los cuales los mas frecuentes son PUSH, COMMIT, PUSH, RESET,  además se creo las ramas principales correctamente para empezar a desarrollar para asi obtener un mejor control de todos los cambios que se vayan realizando.</t>
-  </si>
-  <si>
-    <t>Taller JavaScript Basico-6 JS-JavaScript Basico</t>
+    <t>Capacitacion de Paquete de modulos WebPacket Parte 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instalacion de dependecias de css e implementacion en el ejercicio </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,26 +228,26 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,316 +562,331 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="7"/>
-    <col min="3" max="3" width="51.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="55.85546875" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="7"/>
+    <col min="1" max="2" width="11.42578125" style="5"/>
+    <col min="3" max="3" width="51.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="55.85546875" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" ht="63" x14ac:dyDescent="0.5">
-      <c r="D2" s="8" t="s">
+    <row r="2" spans="3:5" ht="63">
+      <c r="D2" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" ht="16.5" thickBot="1">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="3:5" ht="16.5" thickBot="1">
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="10" t="s">
+    <row r="5" spans="3:5" ht="60" customHeight="1" thickBot="1">
+      <c r="C5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>44732</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="105" customHeight="1" thickBot="1">
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="9">
+        <v>44733</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="3:5" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="11">
-        <v>44733</v>
-      </c>
-      <c r="E6" s="10" t="s">
+    <row r="7" spans="3:5" ht="105" customHeight="1" thickBot="1">
+      <c r="C7" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="9">
+        <v>44734</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="11">
-        <v>44734</v>
-      </c>
-      <c r="E7" s="10" t="s">
+    </row>
+    <row r="8" spans="3:5" ht="105" customHeight="1" thickBot="1">
+      <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="9">
+        <v>44735</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="11">
-        <v>44735</v>
-      </c>
-      <c r="E8" s="10" t="s">
+    </row>
+    <row r="9" spans="3:5" ht="113.25" customHeight="1" thickBot="1">
+      <c r="C9" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="9">
+        <v>44736</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="11">
-        <v>44736</v>
-      </c>
-      <c r="E9" s="10" t="s">
+    </row>
+    <row r="10" spans="3:5" ht="73.5" customHeight="1">
+      <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="3:5" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="9">
+        <v>44737</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="11">
-        <v>44737</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="3:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="3:5" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="3:5" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="3:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="3:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="3:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="3:5" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="3:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="3:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="3:5" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+    </row>
+    <row r="11" spans="3:5" ht="38.25" customHeight="1">
+      <c r="C11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="9">
+        <v>44739</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="15" customHeight="1">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="3:5" ht="34.5" customHeight="1" thickBot="1">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="3:5" ht="15" customHeight="1">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="3:5" ht="36" customHeight="1" thickBot="1">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="3:5" ht="15" customHeight="1">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="3:5" ht="42" customHeight="1" thickBot="1">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="3:5">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="3:5" ht="46.5" customHeight="1" thickBot="1">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="3:5">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="3:5" ht="47.25" customHeight="1" thickBot="1">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="3:5">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="3:5" ht="44.25" customHeight="1" thickBot="1">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="3:5">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="3:5" ht="33" customHeight="1" thickBot="1">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="3:5">
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="3:5" ht="37.5" customHeight="1" thickBot="1">
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="3:5">
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="3:5" ht="45" customHeight="1" thickBot="1">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="3:5">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="3:5" ht="43.5" customHeight="1" thickBot="1">
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="3:5">
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="3:5" ht="44.25" customHeight="1" thickBot="1">
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" spans="3:5">
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="3:5" ht="41.25" customHeight="1" thickBot="1">
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="3:5">
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="3:5" ht="39.75" customHeight="1" thickBot="1">
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" spans="3:5">
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="3:5" ht="45" customHeight="1" thickBot="1">
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" spans="3:5">
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" spans="3:5" ht="36" customHeight="1" thickBot="1">
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" spans="3:5">
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="3:5" ht="48" customHeight="1" thickBot="1">
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+    </row>
+    <row r="44" spans="3:5">
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="3:5" ht="49.5" customHeight="1" thickBot="1">
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+    </row>
+    <row r="46" spans="3:5">
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" spans="3:5" ht="42.75" customHeight="1" thickBot="1">
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+    </row>
+    <row r="48" spans="3:5">
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="3:5" ht="45" customHeight="1" thickBot="1">
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="E40:E41"/>
@@ -870,27 +902,18 @@
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="E38:E39"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>